<commit_message>
Minor changes and corrections to the requirement list
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.requirements/waters-challenge-2019-requirements_v2.xlsx
+++ b/org.panorama-research.waters-2019.requirements/waters-challenge-2019-requirements_v2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WATERS Challenge Artifacts\org.panorama-research.waters-2019.requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A309DD4-6C90-4D6C-93D0-36EB85A90DCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="465" windowWidth="29505" windowHeight="22500"/>
+    <workbookView xWindow="4815" yWindow="465" windowWidth="29505" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -19,25 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Bjoern Koopmann</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D137" authorId="0" shapeId="0">
+    <comment ref="D137" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -145,9 +138,6 @@
     <t>Timing</t>
   </si>
   <si>
-    <t>ECU/Hardware monitor</t>
-  </si>
-  <si>
     <t>Controller</t>
   </si>
   <si>
@@ -215,9 +205,6 @@
   </si>
   <si>
     <t>The system shall prevent unintended breaking.</t>
-  </si>
-  <si>
-    <t>The system shall monitor the ECU status e.g, power supply.</t>
   </si>
   <si>
     <t>The system shall detect road boundaries and the shape of each lane.</t>
@@ -715,7 +702,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1206,11 +1193,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AL149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1232,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>1</v>
@@ -1244,30 +1231,30 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -1275,13 +1262,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -1289,13 +1276,13 @@
         <v>2</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -1303,13 +1290,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -1317,32 +1304,32 @@
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="36"/>
@@ -1351,34 +1338,34 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="27"/>
       <c r="D10" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="12"/>
       <c r="H10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1401,21 +1388,21 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="36"/>
@@ -1424,88 +1411,88 @@
     </row>
     <row r="13" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="38"/>
     </row>
     <row r="17" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="38"/>
@@ -1522,19 +1509,19 @@
     </row>
     <row r="23" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
@@ -1542,74 +1529,74 @@
         <v>4</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
@@ -1618,34 +1605,34 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:26" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="27"/>
       <c r="D31" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="12"/>
       <c r="H31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -1668,21 +1655,21 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
@@ -1691,57 +1678,57 @@
     </row>
     <row r="34" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="38"/>
     </row>
     <row r="36" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="32" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="28"/>
       <c r="D37" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="11"/>
       <c r="H37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -1776,73 +1763,73 @@
     </row>
     <row r="38" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="38"/>
     </row>
     <row r="39" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C40" s="33"/>
       <c r="D40" s="38"/>
     </row>
     <row r="41" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:38" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C42" s="33"/>
       <c r="D42" s="38"/>
     </row>
     <row r="43" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" s="35"/>
       <c r="C44" s="36"/>
@@ -1851,20 +1838,20 @@
     </row>
     <row r="45" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="28"/>
       <c r="D45" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -1899,7 +1886,7 @@
     </row>
     <row r="46" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B46" s="35"/>
       <c r="C46" s="36"/>
@@ -1952,19 +1939,19 @@
     </row>
     <row r="49" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G49" s="19">
         <v>3</v>
@@ -1972,24 +1959,24 @@
     </row>
     <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="28"/>
       <c r="D50" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B51" s="35"/>
       <c r="C51" s="36"/>
@@ -1998,24 +1985,24 @@
     </row>
     <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="28"/>
       <c r="D52" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B53" s="35"/>
       <c r="C53" s="36"/>
@@ -2024,24 +2011,24 @@
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="28"/>
       <c r="D54" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G54" s="11"/>
       <c r="H54" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B55" s="35"/>
       <c r="C55" s="36"/>
@@ -2050,24 +2037,24 @@
     </row>
     <row r="56" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="28"/>
       <c r="D56" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B57" s="35"/>
       <c r="C57" s="36"/>
@@ -2076,24 +2063,24 @@
     </row>
     <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="28"/>
       <c r="D58" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G58" s="11"/>
       <c r="H58" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59" s="35"/>
       <c r="C59" s="36"/>
@@ -2102,47 +2089,47 @@
     </row>
     <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="28"/>
       <c r="D60" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -2153,19 +2140,19 @@
     </row>
     <row r="65" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G65" s="19">
         <v>3</v>
@@ -2173,63 +2160,63 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B70" s="35"/>
       <c r="C70" s="36"/>
@@ -2238,49 +2225,49 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B74" s="35"/>
       <c r="C74" s="36"/>
@@ -2289,35 +2276,35 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B77" s="35"/>
       <c r="C77" s="36"/>
@@ -2326,35 +2313,35 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B80" s="35"/>
       <c r="C80" s="36"/>
@@ -2363,24 +2350,24 @@
     </row>
     <row r="81" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="28"/>
       <c r="D81" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G81" s="11"/>
       <c r="H81" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B82" s="35"/>
       <c r="C82" s="36"/>
@@ -2389,24 +2376,24 @@
     </row>
     <row r="83" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="28"/>
       <c r="D83" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G83" s="11"/>
       <c r="H83" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B84" s="35"/>
       <c r="C84" s="36"/>
@@ -2459,19 +2446,19 @@
     </row>
     <row r="87" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C87" s="30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G87" s="19">
         <v>2</v>
@@ -2479,37 +2466,37 @@
     </row>
     <row r="88" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B88" s="11"/>
       <c r="C88" s="28"/>
       <c r="D88" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="89" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="28"/>
       <c r="D89" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="11"/>
       <c r="H89" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
@@ -2544,7 +2531,7 @@
     </row>
     <row r="90" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B90" s="35"/>
       <c r="C90" s="36"/>
@@ -2553,37 +2540,37 @@
     </row>
     <row r="91" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="28"/>
       <c r="D91" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G91" s="11"/>
       <c r="H91" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="28"/>
       <c r="D92" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="11"/>
       <c r="H92" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
@@ -2618,20 +2605,20 @@
     </row>
     <row r="93" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="28"/>
       <c r="D93" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="11"/>
       <c r="H93" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
@@ -2666,7 +2653,7 @@
     </row>
     <row r="94" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B94" s="35"/>
       <c r="C94" s="36"/>
@@ -2675,34 +2662,34 @@
     </row>
     <row r="95" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A95" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D95" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="28"/>
       <c r="D96" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="11"/>
       <c r="H96" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
@@ -2737,7 +2724,7 @@
     </row>
     <row r="97" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B97" s="35"/>
       <c r="C97" s="36"/>
@@ -2746,34 +2733,34 @@
     </row>
     <row r="98" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D98" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B99" s="11"/>
       <c r="C99" s="28"/>
       <c r="D99" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="11"/>
       <c r="H99" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
@@ -2808,7 +2795,7 @@
     </row>
     <row r="100" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B100" s="35"/>
       <c r="C100" s="36"/>
@@ -2817,21 +2804,21 @@
     </row>
     <row r="101" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A101" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D101" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B102" s="35"/>
       <c r="C102" s="36"/>
@@ -2840,21 +2827,21 @@
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A103" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B104" s="35"/>
       <c r="C104" s="36"/>
@@ -2863,21 +2850,21 @@
     </row>
     <row r="105" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A105" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D105" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B106" s="35"/>
       <c r="C106" s="36"/>
@@ -2886,20 +2873,20 @@
     </row>
     <row r="107" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B107" s="11"/>
       <c r="C107" s="28"/>
       <c r="D107" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="11"/>
       <c r="H107" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
@@ -2934,7 +2921,7 @@
     </row>
     <row r="108" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B108" s="35"/>
       <c r="C108" s="36"/>
@@ -2943,20 +2930,20 @@
     </row>
     <row r="109" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B109" s="11"/>
       <c r="C109" s="28"/>
       <c r="D109" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="11"/>
       <c r="H109" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
@@ -2991,7 +2978,7 @@
     </row>
     <row r="110" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B110" s="35"/>
       <c r="C110" s="36"/>
@@ -3000,20 +2987,20 @@
     </row>
     <row r="111" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B111" s="11"/>
       <c r="C111" s="28"/>
       <c r="D111" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="11"/>
       <c r="H111" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
@@ -3048,7 +3035,7 @@
     </row>
     <row r="112" spans="1:38" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B112" s="35"/>
       <c r="C112" s="36"/>
@@ -3137,195 +3124,195 @@
     </row>
     <row r="115" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C115" s="21"/>
       <c r="D115" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E115" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="116" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A116" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="117" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A117" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="118" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="119" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A119" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="120" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A120" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B120" s="25"/>
       <c r="C120" s="31"/>
       <c r="D120" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="121" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B121" s="25"/>
       <c r="C121" s="31"/>
       <c r="D121" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="122" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A122" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="123" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A123" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A124" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A125" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="127" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A127" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3410,126 +3397,126 @@
     </row>
     <row r="130" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C130" s="21"/>
       <c r="D130" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E130" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="131" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A131" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="132" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B132" s="11"/>
       <c r="C132" s="13"/>
       <c r="D132" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G132" s="11"/>
       <c r="H132" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="133" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B133" s="11"/>
       <c r="C133" s="28"/>
       <c r="D133" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G133" s="11"/>
       <c r="H133" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="134" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A134" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D134" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="135" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D135" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="136" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A136" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="137" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A137" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B137" s="24"/>
       <c r="C137" s="29"/>
       <c r="D137" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="138" spans="1:38" x14ac:dyDescent="0.3">
@@ -3546,32 +3533,32 @@
     </row>
     <row r="140" spans="1:38" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C140" s="21"/>
       <c r="D140" s="23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E140" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="141" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B141" s="11"/>
       <c r="C141" s="28"/>
       <c r="D141" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="11"/>
       <c r="H141" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
@@ -3606,23 +3593,23 @@
     </row>
     <row r="142" spans="1:38" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B142" s="11"/>
       <c r="C142" s="28"/>
       <c r="D142" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="11"/>
       <c r="H142" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
@@ -3656,22 +3643,22 @@
     </row>
     <row r="143" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B143" s="11"/>
       <c r="C143" s="28"/>
       <c r="D143" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G143" s="11"/>
       <c r="H143" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I143" s="2"/>
       <c r="J143" s="2"/>
@@ -3706,22 +3693,22 @@
     </row>
     <row r="144" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B144" s="11"/>
       <c r="C144" s="28"/>
       <c r="D144" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G144" s="11"/>
       <c r="H144" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I144" s="2"/>
       <c r="J144" s="2"/>
@@ -3797,94 +3784,14 @@
     <row r="146" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A146" s="13"/>
     </row>
-    <row r="147" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A147" s="13"/>
-    </row>
-    <row r="148" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="D148" s="8"/>
-      <c r="H148" s="2"/>
-    </row>
-    <row r="150" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A150" s="13"/>
-      <c r="D150" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F150" s="2"/>
-      <c r="G150" s="11"/>
-      <c r="H150" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="151" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="13"/>
-      <c r="B151" s="11"/>
-      <c r="C151" s="28"/>
-      <c r="D151" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F151" s="2"/>
-      <c r="G151" s="11"/>
-      <c r="H151" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I151" s="2"/>
-      <c r="J151" s="2"/>
-      <c r="K151" s="2"/>
-      <c r="L151" s="2"/>
-      <c r="M151" s="2"/>
-      <c r="N151" s="2"/>
-      <c r="O151" s="2"/>
-      <c r="P151" s="2"/>
-      <c r="Q151" s="2"/>
-      <c r="R151" s="2"/>
-      <c r="S151" s="2"/>
-      <c r="T151" s="2"/>
-      <c r="U151" s="2"/>
-      <c r="V151" s="2"/>
-      <c r="W151" s="2"/>
-      <c r="X151" s="2"/>
-      <c r="Y151" s="2"/>
-      <c r="Z151" s="2"/>
-      <c r="AA151" s="2"/>
-      <c r="AB151" s="2"/>
-      <c r="AC151" s="2"/>
-      <c r="AD151" s="2"/>
-      <c r="AE151" s="2"/>
-      <c r="AF151" s="2"/>
-      <c r="AG151" s="2"/>
-      <c r="AH151" s="2"/>
-      <c r="AI151" s="2"/>
-      <c r="AJ151" s="2"/>
-      <c r="AK151" s="2"/>
-      <c r="AL151" s="2"/>
-    </row>
-    <row r="152" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="D152" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F152" s="2"/>
-      <c r="G152" s="11"/>
-      <c r="H152" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D155" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="156" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="D156" s="17" t="s">
-        <v>51</v>
+    <row r="148" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D148" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="149" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="D149" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>